<commit_message>
add missing mapping for kalendere
</commit_message>
<xml_diff>
--- a/src/test/resources/substituttlister/V3_test_kalendere.xlsx
+++ b/src/test/resources/substituttlister/V3_test_kalendere.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aasmund/Documents/mime/Alternativfiler/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dinhanhtuantran/dev/navikt/hm/hm-grunndata-alternativprodukter/src/test/resources/substituttlister/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{302EE027-88BB-C645-A9E5-BE2FB01BBBB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FCB904B-117F-6042-B881-7C6549E721D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="40840" windowHeight="23460" firstSheet="1" activeTab="1" xr2:uid="{DAB7D3D8-04D0-4DD5-9B74-78B882D95CED}"/>
+    <workbookView xWindow="6420" yWindow="700" windowWidth="40840" windowHeight="21100" firstSheet="1" activeTab="1" xr2:uid="{DAB7D3D8-04D0-4DD5-9B74-78B882D95CED}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="243">
   <si>
     <t>Delkontrakt</t>
   </si>
@@ -762,6 +762,12 @@
   </si>
   <si>
     <t>123458</t>
+  </si>
+  <si>
+    <t>MEMOday3</t>
+  </si>
+  <si>
+    <t>313805</t>
   </si>
 </sst>
 </file>
@@ -920,7 +926,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="God" xfId="1" builtinId="26"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2233,10 +2239,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C3485A8-7267-48FD-BE99-693AE922852B}">
-  <dimension ref="A1:J91"/>
+  <dimension ref="A1:J92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M56" sqref="M56"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2283,103 +2289,103 @@
     </row>
     <row r="3" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="C3" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="J3" s="21"/>
+    </row>
+    <row r="4" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="21"/>
-    </row>
-    <row r="4" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="J4" s="21"/>
     </row>
     <row r="5" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="C5" s="2" t="s">
+      <c r="J5" s="21"/>
+    </row>
+    <row r="6" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="21"/>
-    </row>
-    <row r="6" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="J6" s="21"/>
     </row>
     <row r="7" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="C7" s="2" t="s">
+      <c r="J7" s="21"/>
+    </row>
+    <row r="8" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="C8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J7" s="21"/>
-    </row>
-    <row r="8" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="J8" s="21"/>
     </row>
     <row r="9" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="C9" s="2" t="s">
+      <c r="J9" s="21"/>
+    </row>
+    <row r="10" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="C10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="21"/>
-    </row>
-    <row r="10" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="D10" s="2" t="s">
+      <c r="J10" s="21"/>
+    </row>
+    <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="D11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J10" s="21"/>
-    </row>
-    <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="J11" s="21"/>
     </row>
     <row r="12" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="C12" s="2" t="s">
+      <c r="J12" s="21"/>
+    </row>
+    <row r="13" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="C13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J12" s="21"/>
-    </row>
-    <row r="13" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="J13" s="21"/>
     </row>
     <row r="14" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="J14" s="21"/>
+    </row>
+    <row r="15" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="J14" s="21"/>
-    </row>
-    <row r="15" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="D15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="J15" s="21"/>
     </row>
     <row r="16" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="D16" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>25</v>
@@ -2387,23 +2393,23 @@
       <c r="J16" s="21"/>
     </row>
     <row r="17" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="D17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="J17" s="21"/>
     </row>
     <row r="18" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="C18" s="2" t="s">
+      <c r="J18" s="21"/>
+    </row>
+    <row r="19" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="C19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J18" s="21"/>
-    </row>
-    <row r="19" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="D19" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>27</v>
@@ -2411,425 +2417,422 @@
       <c r="J19" s="21"/>
     </row>
     <row r="20" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="D20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="J20" s="21"/>
     </row>
     <row r="21" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="J21" s="21"/>
+    </row>
+    <row r="22" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="J21" s="21"/>
-    </row>
-    <row r="22" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="D22" s="2" t="s">
+      <c r="J22" s="21"/>
+    </row>
+    <row r="23" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="D23" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J22" s="21"/>
-    </row>
-    <row r="23" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="C23" s="2" t="s">
+      <c r="J23" s="21"/>
+    </row>
+    <row r="24" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="C24" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J23" s="21"/>
-    </row>
-    <row r="24" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="J24" s="21"/>
     </row>
     <row r="25" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="C25" s="2" t="s">
+      <c r="J25" s="21"/>
+    </row>
+    <row r="26" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="C26" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="J25" s="21"/>
-    </row>
-    <row r="26" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="D26" s="2" t="s">
+      <c r="J26" s="21"/>
+    </row>
+    <row r="27" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="D27" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="J26" s="21"/>
-    </row>
-    <row r="27" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="J27" s="21"/>
     </row>
     <row r="28" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="C28" s="2" t="s">
+      <c r="J28" s="21"/>
+    </row>
+    <row r="29" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="C29" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J28" s="21"/>
-    </row>
-    <row r="29" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="D29" s="2" t="s">
+      <c r="J29" s="21"/>
+    </row>
+    <row r="30" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="D30" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="E30" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="J29" s="21"/>
-    </row>
-    <row r="30" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="J30" s="21"/>
     </row>
     <row r="31" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="C31" s="2" t="s">
+      <c r="J31" s="21"/>
+    </row>
+    <row r="32" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="C32" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="J31" s="21"/>
-    </row>
-    <row r="32" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="D32" s="2" t="s">
+      <c r="J32" s="21"/>
+    </row>
+    <row r="33" spans="3:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="D33" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="J32" s="21"/>
-    </row>
-    <row r="33" spans="3:10" ht="16" x14ac:dyDescent="0.2">
       <c r="J33" s="21"/>
     </row>
     <row r="34" spans="3:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="C34" s="2" t="s">
+      <c r="J34" s="21"/>
+    </row>
+    <row r="35" spans="3:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="C35" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J34" s="21"/>
-    </row>
-    <row r="35" spans="3:10" ht="16" x14ac:dyDescent="0.2">
       <c r="J35" s="21"/>
     </row>
     <row r="36" spans="3:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="C36" s="2" t="s">
+      <c r="J36" s="21"/>
+    </row>
+    <row r="37" spans="3:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="C37" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="J36" s="21"/>
-    </row>
-    <row r="37" spans="3:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="D37" s="2" t="s">
+      <c r="J37" s="21"/>
+    </row>
+    <row r="38" spans="3:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="D38" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="J37" s="21"/>
-    </row>
-    <row r="38" spans="3:10" ht="16" x14ac:dyDescent="0.2">
       <c r="J38" s="21"/>
     </row>
     <row r="39" spans="3:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="C39" s="2" t="s">
+      <c r="J39" s="21"/>
+    </row>
+    <row r="40" spans="3:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="C40" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D40" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="J39" s="21"/>
-    </row>
-    <row r="40" spans="3:10" ht="16" x14ac:dyDescent="0.2">
       <c r="J40" s="21"/>
     </row>
     <row r="41" spans="3:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="C41" s="2" t="s">
+      <c r="J41" s="21"/>
+    </row>
+    <row r="42" spans="3:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="C42" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D42" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="J41" s="21"/>
-    </row>
-    <row r="42" spans="3:10" ht="16" x14ac:dyDescent="0.2">
       <c r="J42" s="21"/>
     </row>
     <row r="43" spans="3:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="C43" s="2" t="s">
+      <c r="J43" s="21"/>
+    </row>
+    <row r="44" spans="3:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="C44" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D44" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="J43" s="21"/>
-    </row>
-    <row r="44" spans="3:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="D44" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="J44" s="21"/>
     </row>
     <row r="45" spans="3:10" ht="16" x14ac:dyDescent="0.2">
       <c r="D45" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J45" s="21"/>
+    </row>
+    <row r="46" spans="3:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="D46" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="J45" s="21"/>
-    </row>
-    <row r="46" spans="3:10" ht="16" x14ac:dyDescent="0.2">
       <c r="J46" s="21"/>
     </row>
     <row r="47" spans="3:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="C47" s="2" t="s">
+      <c r="J47" s="21"/>
+    </row>
+    <row r="48" spans="3:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="C48" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D48" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="J47" s="21"/>
-    </row>
-    <row r="48" spans="3:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="D48" s="2" t="s">
+      <c r="J48" s="21"/>
+    </row>
+    <row r="49" spans="3:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="D49" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="J48" s="21"/>
-    </row>
-    <row r="49" spans="3:10" ht="16" x14ac:dyDescent="0.2">
       <c r="J49" s="21"/>
     </row>
     <row r="50" spans="3:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="C50" s="2" t="s">
+      <c r="J50" s="21"/>
+    </row>
+    <row r="51" spans="3:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="C51" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="D51" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="J50" s="21"/>
-    </row>
-    <row r="51" spans="3:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="D51" s="2" t="s">
+      <c r="J51" s="21"/>
+    </row>
+    <row r="52" spans="3:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="D52" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="J51" s="21"/>
-    </row>
-    <row r="52" spans="3:10" ht="16" x14ac:dyDescent="0.2">
       <c r="J52" s="21"/>
     </row>
     <row r="53" spans="3:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="C53" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="J53" s="21"/>
     </row>
     <row r="54" spans="3:10" ht="16" x14ac:dyDescent="0.2">
       <c r="C54" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J54" s="21"/>
     </row>
     <row r="55" spans="3:10" ht="16" x14ac:dyDescent="0.2">
       <c r="C55" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J55" s="21"/>
     </row>
     <row r="56" spans="3:10" ht="16" x14ac:dyDescent="0.2">
       <c r="C56" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J56" s="21"/>
+    </row>
+    <row r="57" spans="3:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="C57" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D56" s="2" t="s">
+      <c r="D57" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="J56" s="21"/>
-    </row>
-    <row r="57" spans="3:10" ht="16" x14ac:dyDescent="0.2">
       <c r="J57" s="21"/>
     </row>
     <row r="58" spans="3:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="C58" s="2" t="s">
+      <c r="J58" s="21"/>
+    </row>
+    <row r="59" spans="3:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="C59" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D58" s="2" t="s">
+      <c r="D59" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="J58" s="21"/>
-    </row>
-    <row r="59" spans="3:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="D59" s="2" t="s">
+      <c r="J59" s="21"/>
+    </row>
+    <row r="60" spans="3:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="D60" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="J59" s="21"/>
-    </row>
-    <row r="60" spans="3:10" ht="16" x14ac:dyDescent="0.2">
       <c r="J60" s="21"/>
     </row>
     <row r="61" spans="3:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="C61" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="J61" s="21"/>
     </row>
     <row r="62" spans="3:10" ht="16" x14ac:dyDescent="0.2">
       <c r="C62" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J62" s="21"/>
     </row>
     <row r="63" spans="3:10" ht="16" x14ac:dyDescent="0.2">
       <c r="C63" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J63" s="21"/>
     </row>
     <row r="64" spans="3:10" ht="16" x14ac:dyDescent="0.2">
       <c r="C64" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J64" s="21"/>
+    </row>
+    <row r="65" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="C65" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D64" s="2" t="s">
+      <c r="D65" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="J64" s="21"/>
-    </row>
-    <row r="65" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="J65" s="21"/>
     </row>
     <row r="66" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="C66" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>84</v>
-      </c>
       <c r="J66" s="21"/>
     </row>
     <row r="67" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="C67" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J67" s="21"/>
     </row>
     <row r="68" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="C68" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J68" s="21"/>
     </row>
     <row r="69" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="C69" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J69" s="21"/>
+    </row>
+    <row r="70" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="C70" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D69" s="2" t="s">
+      <c r="D70" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="J69" s="21"/>
-    </row>
-    <row r="70" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="J70" s="21"/>
     </row>
     <row r="71" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A71" s="2" t="s">
+      <c r="J71" s="21"/>
+    </row>
+    <row r="72" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B72" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="C72" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D71" s="2" t="s">
+      <c r="D72" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="J71" s="21"/>
-    </row>
-    <row r="72" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="C72" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="J72" s="21"/>
     </row>
     <row r="73" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="C73" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J73" s="21"/>
     </row>
     <row r="74" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="C74" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J74" s="21"/>
     </row>
     <row r="75" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="C75" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="J75" s="21"/>
+    </row>
+    <row r="76" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="C76" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D75" s="2" t="s">
+      <c r="D76" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="J75" s="21"/>
-    </row>
-    <row r="76" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="J76" s="21"/>
     </row>
     <row r="77" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A77" s="2" t="s">
+      <c r="J77" s="21"/>
+    </row>
+    <row r="78" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A78" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B78" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C77" s="2" t="s">
+      <c r="C78" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D77" s="2" t="s">
+      <c r="D78" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J77" s="21"/>
-    </row>
-    <row r="78" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="C78" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D78" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>27</v>
@@ -2838,10 +2841,10 @@
     </row>
     <row r="79" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="C79" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>27</v>
@@ -2849,26 +2852,26 @@
       <c r="J79" s="21"/>
     </row>
     <row r="80" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="C80" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="J80" s="21"/>
     </row>
     <row r="81" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="C81" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E81" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="J81" s="21"/>
     </row>
     <row r="82" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="C82" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>27</v>
@@ -2876,32 +2879,32 @@
       <c r="J82" s="21"/>
     </row>
     <row r="83" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="C83" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="J83" s="21"/>
     </row>
     <row r="84" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A84" s="2" t="s">
+      <c r="J84" s="21"/>
+    </row>
+    <row r="85" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A85" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B85" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="C85" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D84" s="2" t="s">
+      <c r="D85" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="E84" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J84" s="21"/>
-    </row>
-    <row r="85" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="C85" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>27</v>
@@ -2909,18 +2912,18 @@
       <c r="J85" s="21"/>
     </row>
     <row r="86" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="C86" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="J86" s="21"/>
     </row>
     <row r="87" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="C87" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D87" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="E87" s="2" t="s">
-        <v>122</v>
-      </c>
       <c r="J87" s="21"/>
     </row>
     <row r="88" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -2928,45 +2931,57 @@
         <v>120</v>
       </c>
       <c r="D88" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="J88" s="21"/>
+    </row>
+    <row r="89" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="C89" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D89" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="E88" s="2" t="s">
+      <c r="E89" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J88" s="21"/>
-    </row>
-    <row r="89" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="J89" s="21"/>
     </row>
     <row r="90" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A90" s="2" t="s">
+      <c r="J90" s="21"/>
+    </row>
+    <row r="91" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A91" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="B91" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C90" s="2" t="s">
+      <c r="C91" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D90" s="2" t="s">
+      <c r="D91" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="E90" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J90" s="21"/>
-    </row>
-    <row r="91" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="C91" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D91" s="2" t="s">
-        <v>129</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>27</v>
       </c>
       <c r="J91" s="21"/>
+    </row>
+    <row r="92" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="C92" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J92" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3894,12 +3909,13 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="56a4a40b-dc39-4523-bfc0-6b77a3672d60">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4081,19 +4097,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="56a4a40b-dc39-4523-bfc0-6b77a3672d60">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6084E122-DA70-44DD-8DB1-36165600D3E4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9429DA4-EB02-4F77-87E3-45EA32AEB1B9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="56a4a40b-dc39-4523-bfc0-6b77a3672d60"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4117,11 +4134,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9429DA4-EB02-4F77-87E3-45EA32AEB1B9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6084E122-DA70-44DD-8DB1-36165600D3E4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="56a4a40b-dc39-4523-bfc0-6b77a3672d60"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>